<commit_message>
Adiciona semana 11 do status report
</commit_message>
<xml_diff>
--- a/Documentos/Arquitetura/Uat esboço.xlsx
+++ b/Documentos/Arquitetura/Uat esboço.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="24527"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2773CBC5-A54B-4F98-B3ED-05F5844A2152}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B66B48C8-471B-4B08-B615-32E5C96A36E5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="182" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="213" uniqueCount="87">
   <si>
     <t>Descrição</t>
   </si>
@@ -209,9 +209,6 @@
     <t>Sistema</t>
   </si>
   <si>
-    <t>Caso de teste: Sistema funcionalidades</t>
-  </si>
-  <si>
     <t>Caso de teste: Teste de carga</t>
   </si>
   <si>
@@ -225,6 +222,78 @@
   </si>
   <si>
     <t>O modelo de validação de investidor e dev devem ser os mesmos, assim como os campos em comuns como CPF, NOME, DATA NASC, EMAIL, SENHA e ETC</t>
+  </si>
+  <si>
+    <t>Caso de teste: Sistema funcionalidades Tela Home</t>
+  </si>
+  <si>
+    <t>HM-001</t>
+  </si>
+  <si>
+    <t>HM-002</t>
+  </si>
+  <si>
+    <t>HM-003</t>
+  </si>
+  <si>
+    <t>HM-004</t>
+  </si>
+  <si>
+    <t>HM-005</t>
+  </si>
+  <si>
+    <t>HM-006</t>
+  </si>
+  <si>
+    <t>HM-007</t>
+  </si>
+  <si>
+    <t>HM-008</t>
+  </si>
+  <si>
+    <t>Certificar que os botões no menu estão redirecionando para suas respectivas telas</t>
+  </si>
+  <si>
+    <t>Website Home</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Clique </t>
+  </si>
+  <si>
+    <t>Get</t>
+  </si>
+  <si>
+    <t>Botões</t>
+  </si>
+  <si>
+    <t>Navegar até a página de Home. 1 - Página Home</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Clicar nos botões </t>
+  </si>
+  <si>
+    <t>Devo ser redirecionado para as respectivas telas clicadas</t>
+  </si>
+  <si>
+    <t>João</t>
+  </si>
+  <si>
+    <t>Certificar que a logo no menu retorna para a home</t>
+  </si>
+  <si>
+    <t>Imagem(botão)</t>
+  </si>
+  <si>
+    <t>Navegar até a página de Login. 1 - Página Login</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Clicar nos na imagem da logo </t>
+  </si>
+  <si>
+    <t>Devo ser redirecionado para a home do sistema</t>
+  </si>
+  <si>
+    <t>Certificar que os botões de login(Dev e Investidor) redirecionam para as páginas de login respectivas</t>
   </si>
 </sst>
 </file>
@@ -232,11 +301,11 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
   <numFmts count="5">
-    <numFmt numFmtId="164" formatCode="_-&quot;R$&quot;\ * #,##0.00_-;\-&quot;R$&quot;\ * #,##0.00_-;_-&quot;R$&quot;\ * &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="165" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="166" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="167" formatCode="#_)"/>
-    <numFmt numFmtId="168" formatCode="[&lt;=9999999]###\-####;\(###\)\ ###\-####"/>
+    <numFmt numFmtId="44" formatCode="_-&quot;R$&quot;\ * #,##0.00_-;\-&quot;R$&quot;\ * #,##0.00_-;_-&quot;R$&quot;\ * &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="164" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="165" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="166" formatCode="#_)"/>
+    <numFmt numFmtId="167" formatCode="[&lt;=9999999]###\-####;\(###\)\ ###\-####"/>
   </numFmts>
   <fonts count="28" x14ac:knownFonts="1">
     <font>
@@ -846,26 +915,26 @@
     <xf numFmtId="0" fontId="5" fillId="5" borderId="0" applyBorder="0" applyProtection="0">
       <alignment horizontal="left" indent="1"/>
     </xf>
-    <xf numFmtId="164" fontId="11" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyProtection="0">
+    <xf numFmtId="44" fontId="11" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyProtection="0">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="12" fillId="0" borderId="0" applyFill="0" applyBorder="0" applyProtection="0">
+    <xf numFmtId="44" fontId="12" fillId="0" borderId="0" applyFill="0" applyBorder="0" applyProtection="0">
       <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyProtection="0">
       <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
     </xf>
-    <xf numFmtId="168" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0">
+    <xf numFmtId="167" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="167" fontId="11" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0">
+    <xf numFmtId="166" fontId="11" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0">
       <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="14" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="166" fontId="11" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="165" fontId="11" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="11" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="15" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="16" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -898,7 +967,7 @@
     <xf numFmtId="0" fontId="1" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="42">
+  <cellXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
@@ -944,10 +1013,10 @@
     <xf numFmtId="0" fontId="5" fillId="6" borderId="0" xfId="7" applyFill="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="168" fontId="24" fillId="2" borderId="3" xfId="16" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="24" fillId="2" borderId="3" xfId="16" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="168" fontId="24" fillId="2" borderId="0" xfId="16" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="24" fillId="2" borderId="0" xfId="16" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="25" fillId="0" borderId="2" xfId="2" applyFont="1" applyBorder="1" applyProtection="1">
@@ -962,38 +1031,56 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="12" fillId="36" borderId="1" xfId="13" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="44" fontId="12" fillId="36" borderId="1" xfId="13" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="13" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="13" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="12" fillId="0" borderId="11" xfId="13" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="44" fontId="12" fillId="0" borderId="11" xfId="13" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="12" fillId="0" borderId="1" xfId="13" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="44" fontId="12" fillId="0" borderId="1" xfId="13" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="12" fillId="0" borderId="12" xfId="13" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="44" fontId="12" fillId="0" borderId="12" xfId="13" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="14" fontId="12" fillId="0" borderId="11" xfId="13" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="168" fontId="24" fillId="37" borderId="3" xfId="16" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="24" fillId="37" borderId="3" xfId="16" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="24" fillId="37" borderId="3" xfId="7" applyFont="1" applyFill="1" applyBorder="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="168" fontId="24" fillId="37" borderId="0" xfId="16" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="24" fillId="37" borderId="0" xfId="16" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="24" fillId="37" borderId="0" xfId="7" applyFont="1" applyFill="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="12" fillId="38" borderId="1" xfId="13" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="44" fontId="12" fillId="38" borderId="1" xfId="13" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="44" fontId="12" fillId="6" borderId="1" xfId="13" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="167" fontId="10" fillId="0" borderId="0" xfId="2" applyNumberFormat="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="2" applyProtection="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="2" applyAlignment="1" applyProtection="1">
+      <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="4" xfId="6" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center" indent="2"/>
@@ -1007,22 +1094,7 @@
     <xf numFmtId="0" fontId="27" fillId="37" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="168" fontId="10" fillId="0" borderId="0" xfId="2" applyNumberFormat="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="2" applyProtection="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="2" applyAlignment="1" applyProtection="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="12" fillId="6" borderId="1" xfId="13" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="12" fillId="0" borderId="1" xfId="13" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1098,7 +1170,7 @@
         <family val="2"/>
         <scheme val="minor"/>
       </font>
-      <numFmt numFmtId="164" formatCode="_-&quot;R$&quot;\ * #,##0.00_-;\-&quot;R$&quot;\ * #,##0.00_-;_-&quot;R$&quot;\ * &quot;-&quot;??_-;_-@_-"/>
+      <numFmt numFmtId="34" formatCode="_-&quot;R$&quot;\ * #,##0.00_-;\-&quot;R$&quot;\ * #,##0.00_-;_-&quot;R$&quot;\ * &quot;-&quot;??_-;_-@_-"/>
       <fill>
         <patternFill patternType="none">
           <fgColor indexed="64"/>
@@ -1138,7 +1210,7 @@
         <family val="2"/>
         <scheme val="minor"/>
       </font>
-      <numFmt numFmtId="164" formatCode="_-&quot;R$&quot;\ * #,##0.00_-;\-&quot;R$&quot;\ * #,##0.00_-;_-&quot;R$&quot;\ * &quot;-&quot;??_-;_-@_-"/>
+      <numFmt numFmtId="34" formatCode="_-&quot;R$&quot;\ * #,##0.00_-;\-&quot;R$&quot;\ * #,##0.00_-;_-&quot;R$&quot;\ * &quot;-&quot;??_-;_-@_-"/>
       <fill>
         <patternFill patternType="none">
           <fgColor indexed="64"/>
@@ -1178,7 +1250,7 @@
         <family val="2"/>
         <scheme val="minor"/>
       </font>
-      <numFmt numFmtId="164" formatCode="_-&quot;R$&quot;\ * #,##0.00_-;\-&quot;R$&quot;\ * #,##0.00_-;_-&quot;R$&quot;\ * &quot;-&quot;??_-;_-@_-"/>
+      <numFmt numFmtId="34" formatCode="_-&quot;R$&quot;\ * #,##0.00_-;\-&quot;R$&quot;\ * #,##0.00_-;_-&quot;R$&quot;\ * &quot;-&quot;??_-;_-@_-"/>
       <fill>
         <patternFill patternType="none">
           <fgColor indexed="64"/>
@@ -1218,7 +1290,7 @@
         <family val="2"/>
         <scheme val="minor"/>
       </font>
-      <numFmt numFmtId="164" formatCode="_-&quot;R$&quot;\ * #,##0.00_-;\-&quot;R$&quot;\ * #,##0.00_-;_-&quot;R$&quot;\ * &quot;-&quot;??_-;_-@_-"/>
+      <numFmt numFmtId="34" formatCode="_-&quot;R$&quot;\ * #,##0.00_-;\-&quot;R$&quot;\ * #,##0.00_-;_-&quot;R$&quot;\ * &quot;-&quot;??_-;_-@_-"/>
       <fill>
         <patternFill patternType="none">
           <fgColor indexed="64"/>
@@ -1258,7 +1330,7 @@
         <family val="2"/>
         <scheme val="minor"/>
       </font>
-      <numFmt numFmtId="164" formatCode="_-&quot;R$&quot;\ * #,##0.00_-;\-&quot;R$&quot;\ * #,##0.00_-;_-&quot;R$&quot;\ * &quot;-&quot;??_-;_-@_-"/>
+      <numFmt numFmtId="34" formatCode="_-&quot;R$&quot;\ * #,##0.00_-;\-&quot;R$&quot;\ * #,##0.00_-;_-&quot;R$&quot;\ * &quot;-&quot;??_-;_-@_-"/>
       <fill>
         <patternFill patternType="none">
           <fgColor indexed="64"/>
@@ -1298,7 +1370,7 @@
         <family val="2"/>
         <scheme val="minor"/>
       </font>
-      <numFmt numFmtId="164" formatCode="_-&quot;R$&quot;\ * #,##0.00_-;\-&quot;R$&quot;\ * #,##0.00_-;_-&quot;R$&quot;\ * &quot;-&quot;??_-;_-@_-"/>
+      <numFmt numFmtId="34" formatCode="_-&quot;R$&quot;\ * #,##0.00_-;\-&quot;R$&quot;\ * #,##0.00_-;_-&quot;R$&quot;\ * &quot;-&quot;??_-;_-@_-"/>
       <fill>
         <patternFill patternType="none">
           <fgColor indexed="64"/>
@@ -1338,7 +1410,7 @@
         <family val="2"/>
         <scheme val="minor"/>
       </font>
-      <numFmt numFmtId="164" formatCode="_-&quot;R$&quot;\ * #,##0.00_-;\-&quot;R$&quot;\ * #,##0.00_-;_-&quot;R$&quot;\ * &quot;-&quot;??_-;_-@_-"/>
+      <numFmt numFmtId="34" formatCode="_-&quot;R$&quot;\ * #,##0.00_-;\-&quot;R$&quot;\ * #,##0.00_-;_-&quot;R$&quot;\ * &quot;-&quot;??_-;_-@_-"/>
       <fill>
         <patternFill patternType="none">
           <fgColor indexed="64"/>
@@ -1378,7 +1450,7 @@
         <family val="2"/>
         <scheme val="minor"/>
       </font>
-      <numFmt numFmtId="164" formatCode="_-&quot;R$&quot;\ * #,##0.00_-;\-&quot;R$&quot;\ * #,##0.00_-;_-&quot;R$&quot;\ * &quot;-&quot;??_-;_-@_-"/>
+      <numFmt numFmtId="34" formatCode="_-&quot;R$&quot;\ * #,##0.00_-;\-&quot;R$&quot;\ * #,##0.00_-;_-&quot;R$&quot;\ * &quot;-&quot;??_-;_-@_-"/>
       <fill>
         <patternFill patternType="none">
           <fgColor indexed="64"/>
@@ -1478,7 +1550,7 @@
         <family val="2"/>
         <scheme val="minor"/>
       </font>
-      <numFmt numFmtId="164" formatCode="_-&quot;R$&quot;\ * #,##0.00_-;\-&quot;R$&quot;\ * #,##0.00_-;_-&quot;R$&quot;\ * &quot;-&quot;??_-;_-@_-"/>
+      <numFmt numFmtId="34" formatCode="_-&quot;R$&quot;\ * #,##0.00_-;\-&quot;R$&quot;\ * #,##0.00_-;_-&quot;R$&quot;\ * &quot;-&quot;??_-;_-@_-"/>
       <fill>
         <patternFill patternType="none">
           <fgColor indexed="64"/>
@@ -1518,7 +1590,7 @@
         <family val="2"/>
         <scheme val="minor"/>
       </font>
-      <numFmt numFmtId="164" formatCode="_-&quot;R$&quot;\ * #,##0.00_-;\-&quot;R$&quot;\ * #,##0.00_-;_-&quot;R$&quot;\ * &quot;-&quot;??_-;_-@_-"/>
+      <numFmt numFmtId="34" formatCode="_-&quot;R$&quot;\ * #,##0.00_-;\-&quot;R$&quot;\ * #,##0.00_-;_-&quot;R$&quot;\ * &quot;-&quot;??_-;_-@_-"/>
       <fill>
         <patternFill patternType="none">
           <fgColor indexed="64"/>
@@ -1558,7 +1630,7 @@
         <family val="2"/>
         <scheme val="minor"/>
       </font>
-      <numFmt numFmtId="164" formatCode="_-&quot;R$&quot;\ * #,##0.00_-;\-&quot;R$&quot;\ * #,##0.00_-;_-&quot;R$&quot;\ * &quot;-&quot;??_-;_-@_-"/>
+      <numFmt numFmtId="34" formatCode="_-&quot;R$&quot;\ * #,##0.00_-;\-&quot;R$&quot;\ * #,##0.00_-;_-&quot;R$&quot;\ * &quot;-&quot;??_-;_-@_-"/>
       <fill>
         <patternFill patternType="none">
           <fgColor indexed="64"/>
@@ -1598,7 +1670,7 @@
         <family val="2"/>
         <scheme val="minor"/>
       </font>
-      <numFmt numFmtId="164" formatCode="_-&quot;R$&quot;\ * #,##0.00_-;\-&quot;R$&quot;\ * #,##0.00_-;_-&quot;R$&quot;\ * &quot;-&quot;??_-;_-@_-"/>
+      <numFmt numFmtId="34" formatCode="_-&quot;R$&quot;\ * #,##0.00_-;\-&quot;R$&quot;\ * #,##0.00_-;_-&quot;R$&quot;\ * &quot;-&quot;??_-;_-@_-"/>
       <fill>
         <patternFill patternType="none">
           <fgColor indexed="64"/>
@@ -1638,7 +1710,7 @@
         <family val="2"/>
         <scheme val="minor"/>
       </font>
-      <numFmt numFmtId="164" formatCode="_-&quot;R$&quot;\ * #,##0.00_-;\-&quot;R$&quot;\ * #,##0.00_-;_-&quot;R$&quot;\ * &quot;-&quot;??_-;_-@_-"/>
+      <numFmt numFmtId="34" formatCode="_-&quot;R$&quot;\ * #,##0.00_-;\-&quot;R$&quot;\ * #,##0.00_-;_-&quot;R$&quot;\ * &quot;-&quot;??_-;_-@_-"/>
       <fill>
         <patternFill patternType="none">
           <fgColor indexed="64"/>
@@ -1678,7 +1750,7 @@
         <family val="2"/>
         <scheme val="minor"/>
       </font>
-      <numFmt numFmtId="164" formatCode="_-&quot;R$&quot;\ * #,##0.00_-;\-&quot;R$&quot;\ * #,##0.00_-;_-&quot;R$&quot;\ * &quot;-&quot;??_-;_-@_-"/>
+      <numFmt numFmtId="34" formatCode="_-&quot;R$&quot;\ * #,##0.00_-;\-&quot;R$&quot;\ * #,##0.00_-;_-&quot;R$&quot;\ * &quot;-&quot;??_-;_-@_-"/>
       <fill>
         <patternFill patternType="none">
           <fgColor indexed="64"/>
@@ -1718,7 +1790,7 @@
         <family val="2"/>
         <scheme val="minor"/>
       </font>
-      <numFmt numFmtId="164" formatCode="_-&quot;R$&quot;\ * #,##0.00_-;\-&quot;R$&quot;\ * #,##0.00_-;_-&quot;R$&quot;\ * &quot;-&quot;??_-;_-@_-"/>
+      <numFmt numFmtId="34" formatCode="_-&quot;R$&quot;\ * #,##0.00_-;\-&quot;R$&quot;\ * #,##0.00_-;_-&quot;R$&quot;\ * &quot;-&quot;??_-;_-@_-"/>
       <fill>
         <patternFill patternType="none">
           <fgColor indexed="64"/>
@@ -1758,7 +1830,7 @@
         <family val="2"/>
         <scheme val="minor"/>
       </font>
-      <numFmt numFmtId="164" formatCode="_-&quot;R$&quot;\ * #,##0.00_-;\-&quot;R$&quot;\ * #,##0.00_-;_-&quot;R$&quot;\ * &quot;-&quot;??_-;_-@_-"/>
+      <numFmt numFmtId="34" formatCode="_-&quot;R$&quot;\ * #,##0.00_-;\-&quot;R$&quot;\ * #,##0.00_-;_-&quot;R$&quot;\ * &quot;-&quot;??_-;_-@_-"/>
       <fill>
         <patternFill patternType="none">
           <fgColor indexed="64"/>
@@ -1858,7 +1930,7 @@
         <family val="2"/>
         <scheme val="minor"/>
       </font>
-      <numFmt numFmtId="164" formatCode="_-&quot;R$&quot;\ * #,##0.00_-;\-&quot;R$&quot;\ * #,##0.00_-;_-&quot;R$&quot;\ * &quot;-&quot;??_-;_-@_-"/>
+      <numFmt numFmtId="34" formatCode="_-&quot;R$&quot;\ * #,##0.00_-;\-&quot;R$&quot;\ * #,##0.00_-;_-&quot;R$&quot;\ * &quot;-&quot;??_-;_-@_-"/>
       <fill>
         <patternFill patternType="none">
           <fgColor indexed="64"/>
@@ -1898,7 +1970,7 @@
         <family val="2"/>
         <scheme val="minor"/>
       </font>
-      <numFmt numFmtId="164" formatCode="_-&quot;R$&quot;\ * #,##0.00_-;\-&quot;R$&quot;\ * #,##0.00_-;_-&quot;R$&quot;\ * &quot;-&quot;??_-;_-@_-"/>
+      <numFmt numFmtId="34" formatCode="_-&quot;R$&quot;\ * #,##0.00_-;\-&quot;R$&quot;\ * #,##0.00_-;_-&quot;R$&quot;\ * &quot;-&quot;??_-;_-@_-"/>
       <fill>
         <patternFill patternType="none">
           <fgColor indexed="64"/>
@@ -1938,7 +2010,7 @@
         <family val="2"/>
         <scheme val="minor"/>
       </font>
-      <numFmt numFmtId="164" formatCode="_-&quot;R$&quot;\ * #,##0.00_-;\-&quot;R$&quot;\ * #,##0.00_-;_-&quot;R$&quot;\ * &quot;-&quot;??_-;_-@_-"/>
+      <numFmt numFmtId="34" formatCode="_-&quot;R$&quot;\ * #,##0.00_-;\-&quot;R$&quot;\ * #,##0.00_-;_-&quot;R$&quot;\ * &quot;-&quot;??_-;_-@_-"/>
       <fill>
         <patternFill patternType="none">
           <fgColor indexed="64"/>
@@ -1978,7 +2050,7 @@
         <family val="2"/>
         <scheme val="minor"/>
       </font>
-      <numFmt numFmtId="164" formatCode="_-&quot;R$&quot;\ * #,##0.00_-;\-&quot;R$&quot;\ * #,##0.00_-;_-&quot;R$&quot;\ * &quot;-&quot;??_-;_-@_-"/>
+      <numFmt numFmtId="34" formatCode="_-&quot;R$&quot;\ * #,##0.00_-;\-&quot;R$&quot;\ * #,##0.00_-;_-&quot;R$&quot;\ * &quot;-&quot;??_-;_-@_-"/>
       <fill>
         <patternFill patternType="none">
           <fgColor indexed="64"/>
@@ -2018,7 +2090,7 @@
         <family val="2"/>
         <scheme val="minor"/>
       </font>
-      <numFmt numFmtId="164" formatCode="_-&quot;R$&quot;\ * #,##0.00_-;\-&quot;R$&quot;\ * #,##0.00_-;_-&quot;R$&quot;\ * &quot;-&quot;??_-;_-@_-"/>
+      <numFmt numFmtId="34" formatCode="_-&quot;R$&quot;\ * #,##0.00_-;\-&quot;R$&quot;\ * #,##0.00_-;_-&quot;R$&quot;\ * &quot;-&quot;??_-;_-@_-"/>
       <fill>
         <patternFill patternType="none">
           <fgColor indexed="64"/>
@@ -2058,7 +2130,7 @@
         <family val="2"/>
         <scheme val="minor"/>
       </font>
-      <numFmt numFmtId="164" formatCode="_-&quot;R$&quot;\ * #,##0.00_-;\-&quot;R$&quot;\ * #,##0.00_-;_-&quot;R$&quot;\ * &quot;-&quot;??_-;_-@_-"/>
+      <numFmt numFmtId="34" formatCode="_-&quot;R$&quot;\ * #,##0.00_-;\-&quot;R$&quot;\ * #,##0.00_-;_-&quot;R$&quot;\ * &quot;-&quot;??_-;_-@_-"/>
       <fill>
         <patternFill patternType="none">
           <fgColor indexed="64"/>
@@ -2098,7 +2170,7 @@
         <family val="2"/>
         <scheme val="minor"/>
       </font>
-      <numFmt numFmtId="164" formatCode="_-&quot;R$&quot;\ * #,##0.00_-;\-&quot;R$&quot;\ * #,##0.00_-;_-&quot;R$&quot;\ * &quot;-&quot;??_-;_-@_-"/>
+      <numFmt numFmtId="34" formatCode="_-&quot;R$&quot;\ * #,##0.00_-;\-&quot;R$&quot;\ * #,##0.00_-;_-&quot;R$&quot;\ * &quot;-&quot;??_-;_-@_-"/>
       <fill>
         <patternFill patternType="none">
           <fgColor indexed="64"/>
@@ -2138,7 +2210,7 @@
         <family val="2"/>
         <scheme val="minor"/>
       </font>
-      <numFmt numFmtId="164" formatCode="_-&quot;R$&quot;\ * #,##0.00_-;\-&quot;R$&quot;\ * #,##0.00_-;_-&quot;R$&quot;\ * &quot;-&quot;??_-;_-@_-"/>
+      <numFmt numFmtId="34" formatCode="_-&quot;R$&quot;\ * #,##0.00_-;\-&quot;R$&quot;\ * #,##0.00_-;_-&quot;R$&quot;\ * &quot;-&quot;??_-;_-@_-"/>
       <fill>
         <patternFill patternType="none">
           <fgColor indexed="64"/>
@@ -2238,7 +2310,7 @@
         <family val="2"/>
         <scheme val="minor"/>
       </font>
-      <numFmt numFmtId="164" formatCode="_-&quot;R$&quot;\ * #,##0.00_-;\-&quot;R$&quot;\ * #,##0.00_-;_-&quot;R$&quot;\ * &quot;-&quot;??_-;_-@_-"/>
+      <numFmt numFmtId="34" formatCode="_-&quot;R$&quot;\ * #,##0.00_-;\-&quot;R$&quot;\ * #,##0.00_-;_-&quot;R$&quot;\ * &quot;-&quot;??_-;_-@_-"/>
       <fill>
         <patternFill patternType="none">
           <fgColor indexed="64"/>
@@ -2278,7 +2350,7 @@
         <family val="2"/>
         <scheme val="minor"/>
       </font>
-      <numFmt numFmtId="164" formatCode="_-&quot;R$&quot;\ * #,##0.00_-;\-&quot;R$&quot;\ * #,##0.00_-;_-&quot;R$&quot;\ * &quot;-&quot;??_-;_-@_-"/>
+      <numFmt numFmtId="34" formatCode="_-&quot;R$&quot;\ * #,##0.00_-;\-&quot;R$&quot;\ * #,##0.00_-;_-&quot;R$&quot;\ * &quot;-&quot;??_-;_-@_-"/>
       <fill>
         <patternFill patternType="none">
           <fgColor indexed="64"/>
@@ -2318,7 +2390,7 @@
         <family val="2"/>
         <scheme val="minor"/>
       </font>
-      <numFmt numFmtId="164" formatCode="_-&quot;R$&quot;\ * #,##0.00_-;\-&quot;R$&quot;\ * #,##0.00_-;_-&quot;R$&quot;\ * &quot;-&quot;??_-;_-@_-"/>
+      <numFmt numFmtId="34" formatCode="_-&quot;R$&quot;\ * #,##0.00_-;\-&quot;R$&quot;\ * #,##0.00_-;_-&quot;R$&quot;\ * &quot;-&quot;??_-;_-@_-"/>
       <fill>
         <patternFill patternType="none">
           <fgColor indexed="64"/>
@@ -2358,7 +2430,7 @@
         <family val="2"/>
         <scheme val="minor"/>
       </font>
-      <numFmt numFmtId="164" formatCode="_-&quot;R$&quot;\ * #,##0.00_-;\-&quot;R$&quot;\ * #,##0.00_-;_-&quot;R$&quot;\ * &quot;-&quot;??_-;_-@_-"/>
+      <numFmt numFmtId="34" formatCode="_-&quot;R$&quot;\ * #,##0.00_-;\-&quot;R$&quot;\ * #,##0.00_-;_-&quot;R$&quot;\ * &quot;-&quot;??_-;_-@_-"/>
       <fill>
         <patternFill patternType="none">
           <fgColor indexed="64"/>
@@ -2398,7 +2470,7 @@
         <family val="2"/>
         <scheme val="minor"/>
       </font>
-      <numFmt numFmtId="164" formatCode="_-&quot;R$&quot;\ * #,##0.00_-;\-&quot;R$&quot;\ * #,##0.00_-;_-&quot;R$&quot;\ * &quot;-&quot;??_-;_-@_-"/>
+      <numFmt numFmtId="34" formatCode="_-&quot;R$&quot;\ * #,##0.00_-;\-&quot;R$&quot;\ * #,##0.00_-;_-&quot;R$&quot;\ * &quot;-&quot;??_-;_-@_-"/>
       <fill>
         <patternFill patternType="none">
           <fgColor indexed="64"/>
@@ -2438,7 +2510,7 @@
         <family val="2"/>
         <scheme val="minor"/>
       </font>
-      <numFmt numFmtId="164" formatCode="_-&quot;R$&quot;\ * #,##0.00_-;\-&quot;R$&quot;\ * #,##0.00_-;_-&quot;R$&quot;\ * &quot;-&quot;??_-;_-@_-"/>
+      <numFmt numFmtId="34" formatCode="_-&quot;R$&quot;\ * #,##0.00_-;\-&quot;R$&quot;\ * #,##0.00_-;_-&quot;R$&quot;\ * &quot;-&quot;??_-;_-@_-"/>
       <fill>
         <patternFill patternType="none">
           <fgColor indexed="64"/>
@@ -2478,7 +2550,7 @@
         <family val="2"/>
         <scheme val="minor"/>
       </font>
-      <numFmt numFmtId="164" formatCode="_-&quot;R$&quot;\ * #,##0.00_-;\-&quot;R$&quot;\ * #,##0.00_-;_-&quot;R$&quot;\ * &quot;-&quot;??_-;_-@_-"/>
+      <numFmt numFmtId="34" formatCode="_-&quot;R$&quot;\ * #,##0.00_-;\-&quot;R$&quot;\ * #,##0.00_-;_-&quot;R$&quot;\ * &quot;-&quot;??_-;_-@_-"/>
       <fill>
         <patternFill patternType="none">
           <fgColor indexed="64"/>
@@ -2518,7 +2590,7 @@
         <family val="2"/>
         <scheme val="minor"/>
       </font>
-      <numFmt numFmtId="164" formatCode="_-&quot;R$&quot;\ * #,##0.00_-;\-&quot;R$&quot;\ * #,##0.00_-;_-&quot;R$&quot;\ * &quot;-&quot;??_-;_-@_-"/>
+      <numFmt numFmtId="34" formatCode="_-&quot;R$&quot;\ * #,##0.00_-;\-&quot;R$&quot;\ * #,##0.00_-;_-&quot;R$&quot;\ * &quot;-&quot;??_-;_-@_-"/>
       <fill>
         <patternFill patternType="none">
           <fgColor indexed="64"/>
@@ -2908,11 +2980,11 @@
   <xdr:oneCellAnchor>
     <xdr:from>
       <xdr:col>14</xdr:col>
-      <xdr:colOff>152401</xdr:colOff>
+      <xdr:colOff>581027</xdr:colOff>
       <xdr:row>38</xdr:row>
-      <xdr:rowOff>152401</xdr:rowOff>
+      <xdr:rowOff>47626</xdr:rowOff>
     </xdr:from>
-    <xdr:ext cx="1615756" cy="942974"/>
+    <xdr:ext cx="809624" cy="472506"/>
     <xdr:pic>
       <xdr:nvPicPr>
         <xdr:cNvPr id="6" name="Imagem 5">
@@ -2934,8 +3006,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="23622001" y="3429001"/>
-          <a:ext cx="1615756" cy="942974"/>
+          <a:off x="24050627" y="20526376"/>
+          <a:ext cx="809624" cy="472506"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -3395,8 +3467,8 @@
   </sheetPr>
   <dimension ref="A1:P65"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A13" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A38" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C42" sqref="C42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="33.950000000000003" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -3412,17 +3484,17 @@
   <sheetData>
     <row r="1" spans="1:16" ht="57.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="5"/>
-      <c r="B1" s="32" t="s">
+      <c r="B1" s="38" t="s">
         <v>7</v>
       </c>
-      <c r="C1" s="32"/>
+      <c r="C1" s="38"/>
       <c r="D1" s="2"/>
-      <c r="E1" s="35" t="s">
+      <c r="E1" s="41" t="s">
         <v>33</v>
       </c>
-      <c r="F1" s="35"/>
-      <c r="G1" s="35"/>
-      <c r="H1" s="35"/>
+      <c r="F1" s="41"/>
+      <c r="G1" s="41"/>
+      <c r="H1" s="41"/>
       <c r="I1" s="11"/>
       <c r="J1" s="11"/>
       <c r="K1" s="11"/>
@@ -3433,10 +3505,10 @@
       <c r="P1" s="11"/>
     </row>
     <row r="2" spans="1:16" ht="30" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="33" t="s">
+      <c r="B2" s="39" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="33"/>
+      <c r="C2" s="39"/>
       <c r="D2" s="15" t="s">
         <v>2</v>
       </c>
@@ -3456,10 +3528,10 @@
       <c r="P2" s="13"/>
     </row>
     <row r="3" spans="1:16" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="34" t="s">
+      <c r="B3" s="40" t="s">
         <v>5</v>
       </c>
-      <c r="C3" s="34"/>
+      <c r="C3" s="40"/>
       <c r="D3" s="16" t="s">
         <v>4</v>
       </c>
@@ -3482,10 +3554,10 @@
         <v>3</v>
       </c>
       <c r="C4" s="4"/>
-      <c r="D4" s="36"/>
-      <c r="E4" s="36"/>
-      <c r="F4" s="36"/>
-      <c r="G4" s="36"/>
+      <c r="D4" s="34"/>
+      <c r="E4" s="34"/>
+      <c r="F4" s="34"/>
+      <c r="G4" s="34"/>
       <c r="H4" s="3"/>
       <c r="I4" s="3"/>
       <c r="J4" s="3"/>
@@ -3496,12 +3568,12 @@
       <c r="O4" s="3"/>
     </row>
     <row r="5" spans="1:16" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B5" s="39"/>
-      <c r="C5" s="38"/>
-      <c r="D5" s="36"/>
-      <c r="E5" s="36"/>
-      <c r="F5" s="36"/>
-      <c r="G5" s="36"/>
+      <c r="B5" s="37"/>
+      <c r="C5" s="36"/>
+      <c r="D5" s="34"/>
+      <c r="E5" s="34"/>
+      <c r="F5" s="34"/>
+      <c r="G5" s="34"/>
       <c r="H5" s="3"/>
       <c r="I5" s="3"/>
       <c r="J5" s="3"/>
@@ -3512,12 +3584,12 @@
       <c r="O5" s="3"/>
     </row>
     <row r="6" spans="1:16" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="39"/>
-      <c r="C6" s="38"/>
-      <c r="D6" s="37"/>
-      <c r="E6" s="37"/>
-      <c r="F6" s="37"/>
-      <c r="G6" s="37"/>
+      <c r="B6" s="37"/>
+      <c r="C6" s="36"/>
+      <c r="D6" s="35"/>
+      <c r="E6" s="35"/>
+      <c r="F6" s="35"/>
+      <c r="G6" s="35"/>
       <c r="H6" s="4"/>
       <c r="I6" s="4"/>
       <c r="J6" s="4"/>
@@ -3811,10 +3883,10 @@
     </row>
     <row r="14" spans="1:16" ht="99.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B14" s="19" t="s">
+        <v>59</v>
+      </c>
+      <c r="C14" s="19" t="s">
         <v>60</v>
-      </c>
-      <c r="C14" s="19" t="s">
-        <v>61</v>
       </c>
       <c r="D14" s="20" t="s">
         <v>37</v>
@@ -3828,14 +3900,14 @@
       <c r="G14" s="22" t="s">
         <v>24</v>
       </c>
-      <c r="H14" s="40" t="s">
+      <c r="H14" s="32" t="s">
         <v>26</v>
       </c>
       <c r="I14" s="31" t="s">
+        <v>61</v>
+      </c>
+      <c r="J14" s="33" t="s">
         <v>62</v>
-      </c>
-      <c r="J14" s="41" t="s">
-        <v>63</v>
       </c>
       <c r="K14" s="24"/>
       <c r="L14" s="24"/>
@@ -4251,7 +4323,7 @@
     </row>
     <row r="37" spans="2:16" ht="33.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B37" s="17" t="s">
-        <v>58</v>
+        <v>63</v>
       </c>
       <c r="C37" s="10"/>
       <c r="D37" s="6"/>
@@ -4314,39 +4386,39 @@
         <v>17</v>
       </c>
     </row>
-    <row r="39" spans="2:16" ht="33.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="2:16" ht="45" x14ac:dyDescent="0.25">
       <c r="B39" s="19" t="s">
-        <v>20</v>
+        <v>64</v>
       </c>
       <c r="C39" s="19" t="s">
-        <v>21</v>
+        <v>72</v>
       </c>
       <c r="D39" s="20" t="s">
-        <v>22</v>
+        <v>73</v>
       </c>
       <c r="E39" s="20" t="s">
         <v>36</v>
       </c>
       <c r="F39" s="20" t="s">
-        <v>23</v>
+        <v>74</v>
       </c>
       <c r="G39" s="22" t="s">
-        <v>24</v>
+        <v>75</v>
       </c>
       <c r="H39" s="22" t="s">
-        <v>26</v>
+        <v>76</v>
       </c>
       <c r="I39" s="21" t="s">
-        <v>25</v>
+        <v>77</v>
       </c>
       <c r="J39" s="21" t="s">
-        <v>27</v>
+        <v>78</v>
       </c>
       <c r="K39" s="23" t="s">
-        <v>29</v>
+        <v>79</v>
       </c>
       <c r="L39" s="23" t="s">
-        <v>30</v>
+        <v>80</v>
       </c>
       <c r="M39" s="23" t="s">
         <v>31</v>
@@ -4356,45 +4428,103 @@
       </c>
       <c r="O39" s="23"/>
       <c r="P39" s="26">
-        <v>44497</v>
-      </c>
-    </row>
-    <row r="40" spans="2:16" ht="33.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B40" s="19"/>
-      <c r="C40" s="19"/>
-      <c r="D40" s="20"/>
-      <c r="E40" s="20"/>
-      <c r="F40" s="20"/>
-      <c r="G40" s="22"/>
-      <c r="H40" s="22"/>
-      <c r="I40" s="24"/>
-      <c r="J40" s="24"/>
-      <c r="K40" s="24"/>
-      <c r="L40" s="24"/>
-      <c r="M40" s="24"/>
-      <c r="N40" s="24"/>
+        <v>44516</v>
+      </c>
+    </row>
+    <row r="40" spans="2:16" ht="30" x14ac:dyDescent="0.25">
+      <c r="B40" s="19" t="s">
+        <v>65</v>
+      </c>
+      <c r="C40" s="19" t="s">
+        <v>81</v>
+      </c>
+      <c r="D40" s="20" t="s">
+        <v>22</v>
+      </c>
+      <c r="E40" s="20" t="s">
+        <v>36</v>
+      </c>
+      <c r="F40" s="20" t="s">
+        <v>74</v>
+      </c>
+      <c r="G40" s="22" t="s">
+        <v>75</v>
+      </c>
+      <c r="H40" s="22" t="s">
+        <v>82</v>
+      </c>
+      <c r="I40" s="31" t="s">
+        <v>83</v>
+      </c>
+      <c r="J40" s="31" t="s">
+        <v>84</v>
+      </c>
+      <c r="K40" s="24" t="s">
+        <v>85</v>
+      </c>
+      <c r="L40" s="24" t="s">
+        <v>80</v>
+      </c>
+      <c r="M40" s="24" t="s">
+        <v>31</v>
+      </c>
+      <c r="N40" s="24" t="s">
+        <v>32</v>
+      </c>
       <c r="O40" s="24"/>
-      <c r="P40" s="24"/>
-    </row>
-    <row r="41" spans="2:16" ht="33.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B41" s="19"/>
-      <c r="C41" s="19"/>
-      <c r="D41" s="20"/>
-      <c r="E41" s="20"/>
-      <c r="F41" s="20"/>
-      <c r="G41" s="22"/>
-      <c r="H41" s="9"/>
-      <c r="I41" s="21"/>
-      <c r="J41" s="21"/>
-      <c r="K41" s="24"/>
-      <c r="L41" s="24"/>
-      <c r="M41" s="24"/>
-      <c r="N41" s="24"/>
+      <c r="P40" s="42">
+        <v>44516</v>
+      </c>
+    </row>
+    <row r="41" spans="2:16" ht="45" x14ac:dyDescent="0.25">
+      <c r="B41" s="19" t="s">
+        <v>66</v>
+      </c>
+      <c r="C41" s="19" t="s">
+        <v>86</v>
+      </c>
+      <c r="D41" s="20" t="s">
+        <v>73</v>
+      </c>
+      <c r="E41" s="20" t="s">
+        <v>36</v>
+      </c>
+      <c r="F41" s="20" t="s">
+        <v>74</v>
+      </c>
+      <c r="G41" s="22" t="s">
+        <v>75</v>
+      </c>
+      <c r="H41" s="22" t="s">
+        <v>76</v>
+      </c>
+      <c r="I41" s="21" t="s">
+        <v>77</v>
+      </c>
+      <c r="J41" s="21" t="s">
+        <v>78</v>
+      </c>
+      <c r="K41" s="23" t="s">
+        <v>79</v>
+      </c>
+      <c r="L41" s="24" t="s">
+        <v>80</v>
+      </c>
+      <c r="M41" s="24" t="s">
+        <v>31</v>
+      </c>
+      <c r="N41" s="24" t="s">
+        <v>32</v>
+      </c>
       <c r="O41" s="24"/>
-      <c r="P41" s="24"/>
+      <c r="P41" s="42">
+        <v>44516</v>
+      </c>
     </row>
     <row r="42" spans="2:16" ht="33.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B42" s="19"/>
+      <c r="B42" s="19" t="s">
+        <v>67</v>
+      </c>
       <c r="C42" s="19"/>
       <c r="D42" s="20"/>
       <c r="E42" s="20"/>
@@ -4411,7 +4541,9 @@
       <c r="P42" s="24"/>
     </row>
     <row r="43" spans="2:16" ht="33.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B43" s="19"/>
+      <c r="B43" s="19" t="s">
+        <v>68</v>
+      </c>
       <c r="C43" s="19"/>
       <c r="D43" s="20"/>
       <c r="E43" s="20"/>
@@ -4428,7 +4560,9 @@
       <c r="P43" s="24"/>
     </row>
     <row r="44" spans="2:16" ht="33.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B44" s="19"/>
+      <c r="B44" s="19" t="s">
+        <v>69</v>
+      </c>
       <c r="C44" s="19"/>
       <c r="D44" s="20"/>
       <c r="E44" s="20"/>
@@ -4445,7 +4579,9 @@
       <c r="P44" s="24"/>
     </row>
     <row r="45" spans="2:16" ht="33.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B45" s="19"/>
+      <c r="B45" s="19" t="s">
+        <v>70</v>
+      </c>
       <c r="C45" s="19"/>
       <c r="D45" s="20"/>
       <c r="E45" s="20"/>
@@ -4462,7 +4598,9 @@
       <c r="P45" s="24"/>
     </row>
     <row r="46" spans="2:16" ht="33.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B46" s="19"/>
+      <c r="B46" s="19" t="s">
+        <v>71</v>
+      </c>
       <c r="C46" s="19"/>
       <c r="D46" s="20"/>
       <c r="E46" s="20"/>
@@ -4548,7 +4686,7 @@
     </row>
     <row r="52" spans="2:16" ht="33.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B52" s="17" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C52" s="10"/>
       <c r="D52" s="6"/>
@@ -4880,7 +5018,7 @@
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="L9:L20 L24:L35 L39:L50 L54:L65" xr:uid="{6788DBE9-7B95-4B8C-BE68-509EF6CEB05F}">
       <formula1>"Caio,Vinicius,João,Luis,Lucas G,Lucas F"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E54:E65 E24:E35 E39:E50 E9:E20" xr:uid="{3E10819A-B72F-4549-A018-53739CE06933}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E54:E65 E24:E35 E9:E20 E39:E50" xr:uid="{3E10819A-B72F-4549-A018-53739CE06933}">
       <formula1>"Conteúdo,Bando de dados,Interface,Usabilidade,Compatibilidade,Componentes,Navegação,Configuração,Segurança,Performance,Cargas,Stress"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>